<commit_message>
created bs modal/need to add handlebars to table
</commit_message>
<xml_diff>
--- a/jsd920_class_repo/projects/final_project/public/assets/list-of-URIs.xlsx
+++ b/jsd920_class_repo/projects/final_project/public/assets/list-of-URIs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14160" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="salsa" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>3Pacy6CMa8HPNVfeA3wkPQ</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>https://api.spotify.com/v1/tracks/?ids=0wIEGEWdswpwOnpM3nuwkC,3b2J8pXcrlrGMY4q7zsBtI,3oFwFUxhOgem0hPpFsor1n</t>
+  </si>
+  <si>
+    <t>3Pacy6CMa8HPNVfeA3wkPQ,</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -489,6 +492,11 @@
       </c>
       <c r="D6" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -500,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,7 +563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>